<commit_message>
plots for diyAudio examples
</commit_message>
<xml_diff>
--- a/LD1014D_list.xlsx
+++ b/LD1014D_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="415">
   <si>
     <t xml:space="preserve">LD1014 List (matching without curves)</t>
   </si>
@@ -1175,6 +1175,9 @@
   </si>
   <si>
     <t xml:space="preserve">LD1014D_214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reserved ch</t>
   </si>
   <si>
     <t xml:space="preserve">LD1014D_202</t>
@@ -1533,11 +1536,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ404"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A225" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D245" activeCellId="0" sqref="D245"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A175" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D202" activeCellId="0" sqref="D202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.52"/>
@@ -6416,10 +6419,13 @@
       <c r="C374" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="D374" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="13" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B375" s="2" t="n">
         <v>-1.273</v>
@@ -6427,10 +6433,13 @@
       <c r="C375" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="D375" s="1" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B376" s="2" t="n">
         <v>-1.28</v>
@@ -6441,7 +6450,7 @@
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="13" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B377" s="2" t="n">
         <v>-1.285</v>
@@ -6452,7 +6461,7 @@
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B378" s="2" t="n">
         <v>-1.286</v>
@@ -6463,7 +6472,7 @@
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="13" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B379" s="15" t="n">
         <v>-1.295</v>
@@ -6474,7 +6483,7 @@
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="13" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B380" s="15" t="n">
         <v>-1.296</v>
@@ -6485,7 +6494,7 @@
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="13" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B381" s="2" t="n">
         <v>-1.298</v>
@@ -6496,7 +6505,7 @@
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="13" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B382" s="15" t="n">
         <v>-1.299</v>
@@ -6507,7 +6516,7 @@
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="13" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B383" s="2" t="n">
         <v>-1.303</v>
@@ -6518,7 +6527,7 @@
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="13" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B384" s="15" t="n">
         <v>-1.304</v>
@@ -6529,7 +6538,7 @@
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="13" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B385" s="15" t="n">
         <v>-1.306</v>
@@ -6540,7 +6549,7 @@
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="13" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B386" s="15" t="n">
         <v>-1.307</v>
@@ -6551,7 +6560,7 @@
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="13" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B387" s="2" t="n">
         <v>-1.309</v>
@@ -6562,7 +6571,7 @@
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="13" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B388" s="15" t="n">
         <v>-1.314</v>
@@ -6573,7 +6582,7 @@
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="13" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B389" s="2" t="n">
         <v>-1.323</v>
@@ -6584,7 +6593,7 @@
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="13" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B390" s="2" t="n">
         <v>-1.331</v>
@@ -6595,7 +6604,7 @@
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="13" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B391" s="15" t="n">
         <v>-1.332</v>
@@ -6606,7 +6615,7 @@
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="13" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B392" s="2" t="n">
         <v>-1.335</v>
@@ -6617,7 +6626,7 @@
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="13" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B393" s="15" t="n">
         <v>-1.335</v>
@@ -6628,7 +6637,7 @@
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B394" s="2" t="n">
         <v>-1.343</v>
@@ -6639,7 +6648,7 @@
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B395" s="2" t="n">
         <v>-1.344</v>
@@ -6650,7 +6659,7 @@
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="13" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B396" s="2" t="n">
         <v>-1.346</v>
@@ -6661,7 +6670,7 @@
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="13" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B397" s="2" t="n">
         <v>-1.347</v>
@@ -6672,7 +6681,7 @@
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="13" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B398" s="2" t="n">
         <v>-1.352</v>
@@ -6683,7 +6692,7 @@
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="13" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B399" s="15" t="n">
         <v>-1.362</v>
@@ -6694,7 +6703,7 @@
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="13" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B400" s="15" t="n">
         <v>-1.366</v>
@@ -6705,7 +6714,7 @@
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B401" s="2" t="n">
         <v>-1.375</v>
@@ -6716,7 +6725,7 @@
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="13" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B402" s="2" t="n">
         <v>-1.955</v>
@@ -6725,7 +6734,7 @@
         <v>17</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>